<commit_message>
added more stuff to readme
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonly\OneDrive\Coding Stuff\Project Ideas\prescription fill rate prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonly\Documents\GitHub\prescription-fill-prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="5_{6D7858AC-8405-4013-B6F9-40D3F306D37A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{6D281C1E-6AA5-41B9-8041-955EFD16A28D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D2EFA3-F9F9-4500-89AE-CBF19029A080}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="10">
   <si>
     <t>rx_id</t>
   </si>
   <si>
     <t>patient_id</t>
-  </si>
-  <si>
-    <t>generic_name</t>
   </si>
   <si>
     <t>gender</t>
@@ -51,10 +48,13 @@
     <t>f</t>
   </si>
   <si>
-    <t>apixaban</t>
+    <t>annual_salary</t>
   </si>
   <si>
-    <t>annual_salary</t>
+    <t>entresto</t>
+  </si>
+  <si>
+    <t>brand_name</t>
   </si>
 </sst>
 </file>
@@ -378,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G199"/>
+  <dimension ref="A1:G203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="K203" sqref="K203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -403,19 +403,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -429,7 +429,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1">
         <v>30000</v>
@@ -443,16 +443,18 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
+        <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1">
+        <f>B2+1</f>
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1">
         <v>40000</v>
@@ -466,16 +468,18 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
+        <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1">
+        <f t="shared" ref="B4:B67" si="1">B3+1</f>
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" s="1">
         <v>35000</v>
@@ -489,16 +493,18 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="1">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="1">
         <v>34000</v>
@@ -512,16 +518,18 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="1">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" s="1">
         <v>50000</v>
@@ -535,16 +543,18 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="1">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" s="1">
         <v>60000</v>
@@ -558,16 +568,18 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="1">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" s="1">
         <v>30000</v>
@@ -581,16 +593,18 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="1">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" s="1">
         <v>40000</v>
@@ -604,16 +618,18 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="1">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" s="1">
         <v>35000</v>
@@ -627,16 +643,18 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="1">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" s="1">
         <v>34000</v>
@@ -650,16 +668,18 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="1">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" s="1">
         <v>50000</v>
@@ -673,16 +693,18 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="1">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13" s="1">
         <v>60000</v>
@@ -696,16 +718,18 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="1">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14" s="1">
         <v>30000</v>
@@ -719,16 +743,18 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="1">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15" s="1">
         <v>40000</v>
@@ -742,16 +768,18 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="1">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E16" s="1">
         <v>35000</v>
@@ -765,16 +793,18 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="1">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17" s="1">
         <v>34000</v>
@@ -788,16 +818,18 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="1">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E18" s="1">
         <v>50000</v>
@@ -811,16 +843,18 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="1">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19" s="1">
         <v>60000</v>
@@ -834,16 +868,18 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="1">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E20" s="1">
         <v>70000</v>
@@ -857,16 +893,18 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="1">
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E21" s="1">
         <v>58000</v>
@@ -880,16 +918,18 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="1">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22" s="1">
         <v>54000</v>
@@ -903,16 +943,18 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="1">
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E23" s="1">
         <v>43000</v>
@@ -926,16 +968,18 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="1">
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E24" s="1">
         <v>34000</v>
@@ -949,16 +993,18 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="1">
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E25" s="1">
         <v>50000</v>
@@ -972,16 +1018,18 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="1">
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E26" s="1">
         <v>60000</v>
@@ -995,16 +1043,18 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" s="1">
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E27" s="1">
         <v>70000</v>
@@ -1018,16 +1068,18 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="1">
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E28" s="1">
         <v>58000</v>
@@ -1041,16 +1093,18 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="1">
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E29" s="1">
         <v>54000</v>
@@ -1064,16 +1118,18 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" s="1">
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E30" s="1">
         <v>43000</v>
@@ -1087,16 +1143,18 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="1">
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E31" s="1">
         <v>58000</v>
@@ -1110,16 +1168,18 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" s="1">
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E32" s="1">
         <v>54000</v>
@@ -1133,16 +1193,18 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" s="1">
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E33" s="1">
         <v>43000</v>
@@ -1156,16 +1218,18 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B34" s="1">
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E34" s="1">
         <v>54000</v>
@@ -1179,16 +1243,18 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B35" s="1">
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E35" s="1">
         <v>43000</v>
@@ -1202,16 +1268,18 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B36" s="1">
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E36" s="2">
         <v>100000</v>
@@ -1225,16 +1293,18 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="B37" s="1">
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E37" s="1">
         <v>90000</v>
@@ -1248,16 +1318,18 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="B38" s="1">
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E38" s="1">
         <v>95000</v>
@@ -1271,16 +1343,18 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="B39" s="1">
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E39" s="1">
         <v>97000</v>
@@ -1294,16 +1368,18 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="B40" s="1">
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E40" s="1">
         <v>97000</v>
@@ -1317,16 +1393,18 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="B41" s="1">
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E41" s="1">
         <v>130000</v>
@@ -1340,16 +1418,18 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="B42" s="1">
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E42" s="1">
         <v>140000</v>
@@ -1363,16 +1443,18 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="B43" s="1">
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E43" s="1">
         <v>111000</v>
@@ -1386,16 +1468,18 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="B44" s="1">
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E44" s="1">
         <v>120000</v>
@@ -1409,16 +1493,18 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="B45" s="1">
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E45" s="1">
         <v>140000</v>
@@ -1432,16 +1518,18 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="B46" s="1">
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E46" s="1">
         <v>111000</v>
@@ -1455,16 +1543,18 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="B47" s="1">
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E47" s="1">
         <v>120000</v>
@@ -1478,16 +1568,18 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="B48" s="1">
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E48" s="1">
         <v>30000</v>
@@ -1501,16 +1593,18 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="B49" s="1">
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E49" s="1">
         <v>40000</v>
@@ -1524,19 +1618,21 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="B50" s="1">
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E50" s="1">
-        <v>35000</v>
+        <v>40000</v>
       </c>
       <c r="F50" s="1">
         <v>0</v>
@@ -1547,42 +1643,46 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="B51" s="1">
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E51" s="1">
-        <v>34000</v>
+        <v>35000</v>
       </c>
       <c r="F51" s="1">
         <v>0</v>
       </c>
       <c r="G51" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="B52" s="1">
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E52" s="1">
-        <v>10000</v>
+        <v>34000</v>
       </c>
       <c r="F52" s="1">
         <v>0</v>
@@ -1593,19 +1693,21 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="B53" s="1">
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E53" s="1">
-        <v>11000</v>
+        <v>10000</v>
       </c>
       <c r="F53" s="1">
         <v>0</v>
@@ -1616,19 +1718,21 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="B54" s="1">
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E54" s="1">
-        <v>13000</v>
+        <v>11000</v>
       </c>
       <c r="F54" s="1">
         <v>0</v>
@@ -1639,19 +1743,21 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="B55" s="1">
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E55" s="1">
-        <v>10500</v>
+        <v>13000</v>
       </c>
       <c r="F55" s="1">
         <v>0</v>
@@ -1662,19 +1768,21 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="B56" s="1">
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E56" s="1">
-        <v>15000</v>
+        <v>10500</v>
       </c>
       <c r="F56" s="1">
         <v>0</v>
@@ -1685,19 +1793,21 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="B57" s="1">
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E57" s="1">
-        <v>11500</v>
+        <v>15000</v>
       </c>
       <c r="F57" s="1">
         <v>0</v>
@@ -1708,19 +1818,21 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="B58" s="1">
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E58" s="1">
-        <v>11000</v>
+        <v>11500</v>
       </c>
       <c r="F58" s="1">
         <v>0</v>
@@ -1731,19 +1843,21 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="B59" s="1">
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E59" s="1">
-        <v>13000</v>
+        <v>11000</v>
       </c>
       <c r="F59" s="1">
         <v>0</v>
@@ -1754,19 +1868,21 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
+        <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="B60" s="1">
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E60" s="1">
-        <v>10500</v>
+        <v>13000</v>
       </c>
       <c r="F60" s="1">
         <v>0</v>
@@ -1777,19 +1893,21 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="B61" s="1">
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E61" s="1">
-        <v>15000</v>
+        <v>10500</v>
       </c>
       <c r="F61" s="1">
         <v>0</v>
@@ -1800,19 +1918,21 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="B62" s="1">
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E62" s="1">
-        <v>11500</v>
+        <v>15000</v>
       </c>
       <c r="F62" s="1">
         <v>0</v>
@@ -1823,19 +1943,21 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="B63" s="1">
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E63" s="1">
-        <v>35000</v>
+        <v>11500</v>
       </c>
       <c r="F63" s="1">
         <v>0</v>
@@ -1846,19 +1968,21 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="B64" s="1">
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E64" s="1">
-        <v>34000</v>
+        <v>35000</v>
       </c>
       <c r="F64" s="1">
         <v>0</v>
@@ -1869,19 +1993,21 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="B65" s="1">
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E65" s="1">
-        <v>30000</v>
+        <v>34000</v>
       </c>
       <c r="F65" s="1">
         <v>0</v>
@@ -1892,19 +2018,21 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
+        <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="B66" s="1">
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E66" s="1">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F66" s="1">
         <v>0</v>
@@ -1915,19 +2043,21 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
+        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="B67" s="1">
+        <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E67" s="1">
-        <v>35000</v>
+        <v>40000</v>
       </c>
       <c r="F67" s="1">
         <v>0</v>
@@ -1938,19 +2068,21 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
+        <f t="shared" ref="A68:A131" si="2">A67+1</f>
         <v>67</v>
       </c>
       <c r="B68" s="1">
+        <f t="shared" ref="B68:B131" si="3">B67+1</f>
         <v>67</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E68" s="1">
-        <v>34000</v>
+        <v>35000</v>
       </c>
       <c r="F68" s="1">
         <v>0</v>
@@ -1961,19 +2093,21 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
       <c r="B69" s="1">
+        <f t="shared" si="3"/>
         <v>68</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E69" s="1">
-        <v>10000</v>
+        <v>34000</v>
       </c>
       <c r="F69" s="1">
         <v>0</v>
@@ -1984,19 +2118,21 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
+        <f t="shared" si="2"/>
         <v>69</v>
       </c>
       <c r="B70" s="1">
+        <f t="shared" si="3"/>
         <v>69</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E70" s="1">
-        <v>11000</v>
+        <v>10000</v>
       </c>
       <c r="F70" s="1">
         <v>0</v>
@@ -2007,19 +2143,21 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="B71" s="1">
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E71" s="1">
-        <v>13000</v>
+        <v>11000</v>
       </c>
       <c r="F71" s="1">
         <v>0</v>
@@ -2030,19 +2168,21 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="B72" s="1">
+        <f t="shared" si="3"/>
         <v>71</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E72" s="1">
-        <v>10500</v>
+        <v>13000</v>
       </c>
       <c r="F72" s="1">
         <v>0</v>
@@ -2053,19 +2193,21 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="B73" s="1">
+        <f t="shared" si="3"/>
         <v>72</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E73" s="1">
-        <v>15000</v>
+        <v>10500</v>
       </c>
       <c r="F73" s="1">
         <v>0</v>
@@ -2076,19 +2218,21 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
+        <f t="shared" si="2"/>
         <v>73</v>
       </c>
       <c r="B74" s="1">
+        <f t="shared" si="3"/>
         <v>73</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E74" s="1">
-        <v>11500</v>
+        <v>15000</v>
       </c>
       <c r="F74" s="1">
         <v>0</v>
@@ -2099,19 +2243,21 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="B75" s="1">
+        <f t="shared" si="3"/>
         <v>74</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E75" s="1">
-        <v>11000</v>
+        <v>11500</v>
       </c>
       <c r="F75" s="1">
         <v>0</v>
@@ -2122,19 +2268,21 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="B76" s="1">
+        <f t="shared" si="3"/>
         <v>75</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E76" s="1">
-        <v>13000</v>
+        <v>11000</v>
       </c>
       <c r="F76" s="1">
         <v>0</v>
@@ -2145,19 +2293,21 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
+        <f t="shared" si="2"/>
         <v>76</v>
       </c>
       <c r="B77" s="1">
+        <f t="shared" si="3"/>
         <v>76</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E77" s="1">
-        <v>10500</v>
+        <v>13000</v>
       </c>
       <c r="F77" s="1">
         <v>0</v>
@@ -2168,19 +2318,21 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="B78" s="1">
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E78" s="1">
-        <v>15000</v>
+        <v>10500</v>
       </c>
       <c r="F78" s="1">
         <v>0</v>
@@ -2191,19 +2343,21 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
+        <f t="shared" si="2"/>
         <v>78</v>
       </c>
       <c r="B79" s="1">
+        <f t="shared" si="3"/>
         <v>78</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E79" s="1">
-        <v>11500</v>
+        <v>15000</v>
       </c>
       <c r="F79" s="1">
         <v>0</v>
@@ -2214,19 +2368,21 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
+        <f t="shared" si="2"/>
         <v>79</v>
       </c>
       <c r="B80" s="1">
+        <f t="shared" si="3"/>
         <v>79</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E80" s="1">
-        <v>35000</v>
+        <v>11500</v>
       </c>
       <c r="F80" s="1">
         <v>0</v>
@@ -2237,19 +2393,21 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="B81" s="1">
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E81" s="1">
-        <v>34000</v>
+        <v>35000</v>
       </c>
       <c r="F81" s="1">
         <v>0</v>
@@ -2260,19 +2418,21 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="B82" s="1">
+        <f t="shared" si="3"/>
         <v>81</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E82" s="1">
-        <v>25000</v>
+        <v>34000</v>
       </c>
       <c r="F82" s="1">
         <v>0</v>
@@ -2283,19 +2443,21 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
+        <f t="shared" si="2"/>
         <v>82</v>
       </c>
       <c r="B83" s="1">
+        <f t="shared" si="3"/>
         <v>82</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E83" s="1">
-        <v>27000</v>
+        <v>25000</v>
       </c>
       <c r="F83" s="1">
         <v>0</v>
@@ -2306,19 +2468,21 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
+        <f t="shared" si="2"/>
         <v>83</v>
       </c>
       <c r="B84" s="1">
+        <f t="shared" si="3"/>
         <v>83</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E84" s="1">
-        <v>29000</v>
+        <v>27000</v>
       </c>
       <c r="F84" s="1">
         <v>0</v>
@@ -2329,19 +2493,21 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
       <c r="B85" s="1">
+        <f t="shared" si="3"/>
         <v>84</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E85" s="1">
-        <v>27007</v>
+        <v>29000</v>
       </c>
       <c r="F85" s="1">
         <v>0</v>
@@ -2352,19 +2518,21 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="B86" s="1">
+        <f t="shared" si="3"/>
         <v>85</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E86" s="1">
-        <v>27500</v>
+        <v>27007</v>
       </c>
       <c r="F86" s="1">
         <v>0</v>
@@ -2375,19 +2543,21 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
+        <f t="shared" si="2"/>
         <v>86</v>
       </c>
       <c r="B87" s="1">
+        <f t="shared" si="3"/>
         <v>86</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E87" s="1">
-        <v>24890</v>
+        <v>27500</v>
       </c>
       <c r="F87" s="1">
         <v>0</v>
@@ -2398,19 +2568,21 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
+        <f t="shared" si="2"/>
         <v>87</v>
       </c>
       <c r="B88" s="1">
+        <f t="shared" si="3"/>
         <v>87</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E88" s="1">
-        <v>22000</v>
+        <v>24890</v>
       </c>
       <c r="F88" s="1">
         <v>0</v>
@@ -2421,19 +2593,21 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
+        <f t="shared" si="2"/>
         <v>88</v>
       </c>
       <c r="B89" s="1">
+        <f t="shared" si="3"/>
         <v>88</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E89" s="1">
-        <v>26589</v>
+        <v>22000</v>
       </c>
       <c r="F89" s="1">
         <v>0</v>
@@ -2444,22 +2618,24 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
+        <f t="shared" si="2"/>
         <v>89</v>
       </c>
       <c r="B90" s="1">
+        <f t="shared" si="3"/>
         <v>89</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E90" s="1">
-        <v>3000</v>
+        <v>26589</v>
       </c>
       <c r="F90" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G90" s="1">
         <v>0</v>
@@ -2467,19 +2643,21 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="B91" s="1">
+        <f t="shared" si="3"/>
         <v>90</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E91" s="1">
-        <v>7700</v>
+        <v>3000</v>
       </c>
       <c r="F91" s="1">
         <v>1</v>
@@ -2490,19 +2668,21 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
+        <f t="shared" si="2"/>
         <v>91</v>
       </c>
       <c r="B92" s="1">
+        <f t="shared" si="3"/>
         <v>91</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E92" s="1">
-        <v>7000</v>
+        <v>7700</v>
       </c>
       <c r="F92" s="1">
         <v>1</v>
@@ -2513,19 +2693,21 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
+        <f t="shared" si="2"/>
         <v>92</v>
       </c>
       <c r="B93" s="1">
+        <f t="shared" si="3"/>
         <v>92</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E93" s="1">
-        <v>8000</v>
+        <v>7000</v>
       </c>
       <c r="F93" s="1">
         <v>1</v>
@@ -2536,19 +2718,21 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
+        <f t="shared" si="2"/>
         <v>93</v>
       </c>
       <c r="B94" s="1">
+        <f t="shared" si="3"/>
         <v>93</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E94" s="1">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="F94" s="1">
         <v>1</v>
@@ -2559,19 +2743,21 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
+        <f t="shared" si="2"/>
         <v>94</v>
       </c>
       <c r="B95" s="1">
+        <f t="shared" si="3"/>
         <v>94</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E95" s="1">
-        <v>8600</v>
+        <v>7500</v>
       </c>
       <c r="F95" s="1">
         <v>1</v>
@@ -2582,19 +2768,21 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
+        <f t="shared" si="2"/>
         <v>95</v>
       </c>
       <c r="B96" s="1">
+        <f t="shared" si="3"/>
         <v>95</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E96" s="1">
-        <v>8000</v>
+        <v>8600</v>
       </c>
       <c r="F96" s="1">
         <v>1</v>
@@ -2605,19 +2793,21 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
+        <f t="shared" si="2"/>
         <v>96</v>
       </c>
       <c r="B97" s="1">
+        <f t="shared" si="3"/>
         <v>96</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E97" s="1">
-        <v>9000</v>
+        <v>8000</v>
       </c>
       <c r="F97" s="1">
         <v>1</v>
@@ -2628,19 +2818,21 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
+        <f t="shared" si="2"/>
         <v>97</v>
       </c>
       <c r="B98" s="1">
+        <f t="shared" si="3"/>
         <v>97</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E98" s="1">
-        <v>10000</v>
+        <v>9000</v>
       </c>
       <c r="F98" s="1">
         <v>1</v>
@@ -2651,19 +2843,21 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
+        <f t="shared" si="2"/>
         <v>98</v>
       </c>
       <c r="B99" s="1">
+        <f t="shared" si="3"/>
         <v>98</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E99" s="1">
-        <v>11000</v>
+        <v>10000</v>
       </c>
       <c r="F99" s="1">
         <v>1</v>
@@ -2674,19 +2868,21 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
+        <f t="shared" si="2"/>
         <v>99</v>
       </c>
       <c r="B100" s="1">
+        <f t="shared" si="3"/>
         <v>99</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E100" s="1">
-        <v>8000</v>
+        <v>11000</v>
       </c>
       <c r="F100" s="1">
         <v>1</v>
@@ -2697,42 +2893,46 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="B101" s="1">
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E101" s="1">
-        <v>30000</v>
+        <v>8000</v>
       </c>
       <c r="F101" s="1">
         <v>1</v>
       </c>
       <c r="G101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
+        <f t="shared" si="2"/>
         <v>101</v>
       </c>
       <c r="B102" s="1">
+        <f t="shared" si="3"/>
         <v>101</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E102" s="1">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F102" s="1">
         <v>1</v>
@@ -2743,19 +2943,21 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
+        <f t="shared" si="2"/>
         <v>102</v>
       </c>
       <c r="B103" s="1">
+        <f t="shared" si="3"/>
         <v>102</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E103" s="1">
-        <v>35000</v>
+        <v>40000</v>
       </c>
       <c r="F103" s="1">
         <v>1</v>
@@ -2766,19 +2968,21 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
+        <f t="shared" si="2"/>
         <v>103</v>
       </c>
       <c r="B104" s="1">
+        <f t="shared" si="3"/>
         <v>103</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E104" s="1">
-        <v>34000</v>
+        <v>35000</v>
       </c>
       <c r="F104" s="1">
         <v>1</v>
@@ -2789,19 +2993,21 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
+        <f t="shared" si="2"/>
         <v>104</v>
       </c>
       <c r="B105" s="1">
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E105" s="1">
-        <v>50000</v>
+        <v>34000</v>
       </c>
       <c r="F105" s="1">
         <v>1</v>
@@ -2812,19 +3018,21 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
+        <f t="shared" si="2"/>
         <v>105</v>
       </c>
       <c r="B106" s="1">
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E106" s="1">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F106" s="1">
         <v>1</v>
@@ -2835,19 +3043,21 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
+        <f t="shared" si="2"/>
         <v>106</v>
       </c>
       <c r="B107" s="1">
+        <f t="shared" si="3"/>
         <v>106</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E107" s="1">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="F107" s="1">
         <v>1</v>
@@ -2858,19 +3068,21 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
+        <f t="shared" si="2"/>
         <v>107</v>
       </c>
       <c r="B108" s="1">
+        <f t="shared" si="3"/>
         <v>107</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E108" s="1">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F108" s="1">
         <v>1</v>
@@ -2881,19 +3093,21 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
+        <f t="shared" si="2"/>
         <v>108</v>
       </c>
       <c r="B109" s="1">
+        <f t="shared" si="3"/>
         <v>108</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E109" s="1">
-        <v>35000</v>
+        <v>40000</v>
       </c>
       <c r="F109" s="1">
         <v>1</v>
@@ -2904,19 +3118,21 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
+        <f t="shared" si="2"/>
         <v>109</v>
       </c>
       <c r="B110" s="1">
+        <f t="shared" si="3"/>
         <v>109</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E110" s="1">
-        <v>34000</v>
+        <v>35000</v>
       </c>
       <c r="F110" s="1">
         <v>1</v>
@@ -2927,19 +3143,21 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
       <c r="B111" s="1">
+        <f t="shared" si="3"/>
         <v>110</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E111" s="1">
-        <v>50000</v>
+        <v>34000</v>
       </c>
       <c r="F111" s="1">
         <v>1</v>
@@ -2950,19 +3168,21 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
+        <f t="shared" si="2"/>
         <v>111</v>
       </c>
       <c r="B112" s="1">
+        <f t="shared" si="3"/>
         <v>111</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E112" s="1">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F112" s="1">
         <v>1</v>
@@ -2973,19 +3193,21 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
+        <f t="shared" si="2"/>
         <v>112</v>
       </c>
       <c r="B113" s="1">
+        <f t="shared" si="3"/>
         <v>112</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E113" s="1">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="F113" s="1">
         <v>1</v>
@@ -2996,19 +3218,21 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
+        <f t="shared" si="2"/>
         <v>113</v>
       </c>
       <c r="B114" s="1">
+        <f t="shared" si="3"/>
         <v>113</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E114" s="1">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F114" s="1">
         <v>1</v>
@@ -3019,19 +3243,21 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
+        <f t="shared" si="2"/>
         <v>114</v>
       </c>
       <c r="B115" s="1">
+        <f t="shared" si="3"/>
         <v>114</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E115" s="1">
-        <v>35000</v>
+        <v>40000</v>
       </c>
       <c r="F115" s="1">
         <v>1</v>
@@ -3042,19 +3268,21 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
+        <f t="shared" si="2"/>
         <v>115</v>
       </c>
       <c r="B116" s="1">
+        <f t="shared" si="3"/>
         <v>115</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E116" s="1">
-        <v>34000</v>
+        <v>35000</v>
       </c>
       <c r="F116" s="1">
         <v>1</v>
@@ -3065,19 +3293,21 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
+        <f t="shared" si="2"/>
         <v>116</v>
       </c>
       <c r="B117" s="1">
+        <f t="shared" si="3"/>
         <v>116</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E117" s="1">
-        <v>50000</v>
+        <v>34000</v>
       </c>
       <c r="F117" s="1">
         <v>1</v>
@@ -3088,19 +3318,21 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
+        <f t="shared" si="2"/>
         <v>117</v>
       </c>
       <c r="B118" s="1">
+        <f t="shared" si="3"/>
         <v>117</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E118" s="1">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F118" s="1">
         <v>1</v>
@@ -3111,19 +3343,21 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="B119" s="1">
+        <f t="shared" si="3"/>
         <v>118</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E119" s="1">
-        <v>70000</v>
+        <v>60000</v>
       </c>
       <c r="F119" s="1">
         <v>1</v>
@@ -3134,19 +3368,21 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
+        <f t="shared" si="2"/>
         <v>119</v>
       </c>
       <c r="B120" s="1">
+        <f t="shared" si="3"/>
         <v>119</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E120" s="1">
-        <v>58000</v>
+        <v>70000</v>
       </c>
       <c r="F120" s="1">
         <v>1</v>
@@ -3157,19 +3393,21 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
       <c r="B121" s="1">
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E121" s="1">
-        <v>54000</v>
+        <v>58000</v>
       </c>
       <c r="F121" s="1">
         <v>1</v>
@@ -3180,19 +3418,21 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
+        <f t="shared" si="2"/>
         <v>121</v>
       </c>
       <c r="B122" s="1">
+        <f t="shared" si="3"/>
         <v>121</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E122" s="1">
-        <v>43000</v>
+        <v>54000</v>
       </c>
       <c r="F122" s="1">
         <v>1</v>
@@ -3203,19 +3443,21 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
+        <f t="shared" si="2"/>
         <v>122</v>
       </c>
       <c r="B123" s="1">
+        <f t="shared" si="3"/>
         <v>122</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E123" s="1">
-        <v>34000</v>
+        <v>43000</v>
       </c>
       <c r="F123" s="1">
         <v>1</v>
@@ -3226,19 +3468,21 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
+        <f t="shared" si="2"/>
         <v>123</v>
       </c>
       <c r="B124" s="1">
+        <f t="shared" si="3"/>
         <v>123</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E124" s="1">
-        <v>50000</v>
+        <v>34000</v>
       </c>
       <c r="F124" s="1">
         <v>1</v>
@@ -3249,19 +3493,21 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
+        <f t="shared" si="2"/>
         <v>124</v>
       </c>
       <c r="B125" s="1">
+        <f t="shared" si="3"/>
         <v>124</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E125" s="1">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F125" s="1">
         <v>1</v>
@@ -3272,19 +3518,21 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
+        <f t="shared" si="2"/>
         <v>125</v>
       </c>
       <c r="B126" s="1">
+        <f t="shared" si="3"/>
         <v>125</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E126" s="1">
-        <v>70000</v>
+        <v>60000</v>
       </c>
       <c r="F126" s="1">
         <v>1</v>
@@ -3295,19 +3543,21 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
+        <f t="shared" si="2"/>
         <v>126</v>
       </c>
       <c r="B127" s="1">
+        <f t="shared" si="3"/>
         <v>126</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E127" s="1">
-        <v>58000</v>
+        <v>70000</v>
       </c>
       <c r="F127" s="1">
         <v>1</v>
@@ -3318,19 +3568,21 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
+        <f t="shared" si="2"/>
         <v>127</v>
       </c>
       <c r="B128" s="1">
+        <f t="shared" si="3"/>
         <v>127</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E128" s="1">
-        <v>54000</v>
+        <v>58000</v>
       </c>
       <c r="F128" s="1">
         <v>1</v>
@@ -3341,19 +3593,21 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
+        <f t="shared" si="2"/>
         <v>128</v>
       </c>
       <c r="B129" s="1">
+        <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E129" s="1">
-        <v>43000</v>
+        <v>54000</v>
       </c>
       <c r="F129" s="1">
         <v>1</v>
@@ -3364,19 +3618,21 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
+        <f t="shared" si="2"/>
         <v>129</v>
       </c>
       <c r="B130" s="1">
+        <f t="shared" si="3"/>
         <v>129</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E130" s="1">
-        <v>58000</v>
+        <v>43000</v>
       </c>
       <c r="F130" s="1">
         <v>1</v>
@@ -3387,19 +3643,21 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
+        <f t="shared" si="2"/>
         <v>130</v>
       </c>
       <c r="B131" s="1">
+        <f t="shared" si="3"/>
         <v>130</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E131" s="1">
-        <v>54000</v>
+        <v>58000</v>
       </c>
       <c r="F131" s="1">
         <v>1</v>
@@ -3410,19 +3668,21 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
+        <f t="shared" ref="A132:A195" si="4">A131+1</f>
         <v>131</v>
       </c>
       <c r="B132" s="1">
+        <f t="shared" ref="B132:B195" si="5">B131+1</f>
         <v>131</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E132" s="1">
-        <v>43000</v>
+        <v>54000</v>
       </c>
       <c r="F132" s="1">
         <v>1</v>
@@ -3433,19 +3693,21 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
+        <f t="shared" si="4"/>
         <v>132</v>
       </c>
       <c r="B133" s="1">
+        <f t="shared" si="5"/>
         <v>132</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E133" s="1">
-        <v>54000</v>
+        <v>43000</v>
       </c>
       <c r="F133" s="1">
         <v>1</v>
@@ -3456,19 +3718,21 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
+        <f t="shared" si="4"/>
         <v>133</v>
       </c>
       <c r="B134" s="1">
+        <f t="shared" si="5"/>
         <v>133</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E134" s="1">
-        <v>43000</v>
+        <v>54000</v>
       </c>
       <c r="F134" s="1">
         <v>1</v>
@@ -3479,22 +3743,24 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
+        <f t="shared" si="4"/>
         <v>134</v>
       </c>
       <c r="B135" s="1">
+        <f t="shared" si="5"/>
         <v>134</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E135" s="2">
-        <v>100000</v>
+        <v>4</v>
+      </c>
+      <c r="E135" s="1">
+        <v>43000</v>
       </c>
       <c r="F135" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G135" s="1">
         <v>1</v>
@@ -3502,19 +3768,21 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
+        <f t="shared" si="4"/>
         <v>135</v>
       </c>
       <c r="B136" s="1">
+        <f t="shared" si="5"/>
         <v>135</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E136" s="1">
-        <v>90000</v>
+        <v>6</v>
+      </c>
+      <c r="E136" s="2">
+        <v>100000</v>
       </c>
       <c r="F136" s="1">
         <v>0</v>
@@ -3525,19 +3793,21 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
+        <f t="shared" si="4"/>
         <v>136</v>
       </c>
       <c r="B137" s="1">
+        <f t="shared" si="5"/>
         <v>136</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E137" s="1">
-        <v>95000</v>
+        <v>90000</v>
       </c>
       <c r="F137" s="1">
         <v>0</v>
@@ -3548,19 +3818,21 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
+        <f t="shared" si="4"/>
         <v>137</v>
       </c>
       <c r="B138" s="1">
+        <f t="shared" si="5"/>
         <v>137</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E138" s="1">
-        <v>97000</v>
+        <v>95000</v>
       </c>
       <c r="F138" s="1">
         <v>0</v>
@@ -3571,16 +3843,18 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
+        <f t="shared" si="4"/>
         <v>138</v>
       </c>
       <c r="B139" s="1">
+        <f t="shared" si="5"/>
         <v>138</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E139" s="1">
         <v>97000</v>
@@ -3594,19 +3868,21 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
+        <f t="shared" si="4"/>
         <v>139</v>
       </c>
       <c r="B140" s="1">
+        <f t="shared" si="5"/>
         <v>139</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E140" s="1">
-        <v>130000</v>
+        <v>97000</v>
       </c>
       <c r="F140" s="1">
         <v>0</v>
@@ -3617,19 +3893,21 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
+        <f t="shared" si="4"/>
         <v>140</v>
       </c>
       <c r="B141" s="1">
+        <f t="shared" si="5"/>
         <v>140</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E141" s="1">
-        <v>140000</v>
+        <v>130000</v>
       </c>
       <c r="F141" s="1">
         <v>0</v>
@@ -3640,19 +3918,21 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
+        <f t="shared" si="4"/>
         <v>141</v>
       </c>
       <c r="B142" s="1">
+        <f t="shared" si="5"/>
         <v>141</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E142" s="1">
-        <v>111000</v>
+        <v>140000</v>
       </c>
       <c r="F142" s="1">
         <v>0</v>
@@ -3663,19 +3943,21 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
+        <f t="shared" si="4"/>
         <v>142</v>
       </c>
       <c r="B143" s="1">
+        <f t="shared" si="5"/>
         <v>142</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E143" s="1">
-        <v>120000</v>
+        <v>111000</v>
       </c>
       <c r="F143" s="1">
         <v>0</v>
@@ -3686,19 +3968,21 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
+        <f t="shared" si="4"/>
         <v>143</v>
       </c>
       <c r="B144" s="1">
+        <f t="shared" si="5"/>
         <v>143</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E144" s="1">
-        <v>140000</v>
+        <v>120000</v>
       </c>
       <c r="F144" s="1">
         <v>0</v>
@@ -3709,19 +3993,21 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
+        <f t="shared" si="4"/>
         <v>144</v>
       </c>
       <c r="B145" s="1">
+        <f t="shared" si="5"/>
         <v>144</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E145" s="1">
-        <v>111000</v>
+        <v>140000</v>
       </c>
       <c r="F145" s="1">
         <v>0</v>
@@ -3732,19 +4018,21 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
+        <f t="shared" si="4"/>
         <v>145</v>
       </c>
       <c r="B146" s="1">
+        <f t="shared" si="5"/>
         <v>145</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E146" s="1">
-        <v>120000</v>
+        <v>111000</v>
       </c>
       <c r="F146" s="1">
         <v>0</v>
@@ -3755,19 +4043,21 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
+        <f t="shared" si="4"/>
         <v>146</v>
       </c>
       <c r="B147" s="1">
+        <f t="shared" si="5"/>
         <v>146</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E147" s="1">
-        <v>30000</v>
+        <v>120000</v>
       </c>
       <c r="F147" s="1">
         <v>0</v>
@@ -3778,19 +4068,21 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
+        <f t="shared" si="4"/>
         <v>147</v>
       </c>
       <c r="B148" s="1">
+        <f t="shared" si="5"/>
         <v>147</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E148" s="1">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F148" s="1">
         <v>0</v>
@@ -3801,19 +4093,21 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
+        <f t="shared" si="4"/>
         <v>148</v>
       </c>
       <c r="B149" s="1">
+        <f t="shared" si="5"/>
         <v>148</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E149" s="1">
-        <v>35000</v>
+        <v>40000</v>
       </c>
       <c r="F149" s="1">
         <v>0</v>
@@ -3824,42 +4118,46 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
+        <f t="shared" si="4"/>
         <v>149</v>
       </c>
       <c r="B150" s="1">
+        <f t="shared" si="5"/>
         <v>149</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E150" s="1">
-        <v>34000</v>
+        <v>35000</v>
       </c>
       <c r="F150" s="1">
         <v>0</v>
       </c>
       <c r="G150" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
       <c r="B151" s="1">
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E151" s="1">
-        <v>10000</v>
+        <v>34000</v>
       </c>
       <c r="F151" s="1">
         <v>0</v>
@@ -3870,19 +4168,21 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
+        <f t="shared" si="4"/>
         <v>151</v>
       </c>
       <c r="B152" s="1">
+        <f t="shared" si="5"/>
         <v>151</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E152" s="1">
-        <v>11000</v>
+        <v>10000</v>
       </c>
       <c r="F152" s="1">
         <v>0</v>
@@ -3893,19 +4193,21 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
+        <f t="shared" si="4"/>
         <v>152</v>
       </c>
       <c r="B153" s="1">
+        <f t="shared" si="5"/>
         <v>152</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E153" s="1">
-        <v>13000</v>
+        <v>11000</v>
       </c>
       <c r="F153" s="1">
         <v>0</v>
@@ -3916,19 +4218,21 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
+        <f t="shared" si="4"/>
         <v>153</v>
       </c>
       <c r="B154" s="1">
+        <f t="shared" si="5"/>
         <v>153</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E154" s="1">
-        <v>10500</v>
+        <v>13000</v>
       </c>
       <c r="F154" s="1">
         <v>0</v>
@@ -3939,19 +4243,21 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
+        <f t="shared" si="4"/>
         <v>154</v>
       </c>
       <c r="B155" s="1">
+        <f t="shared" si="5"/>
         <v>154</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E155" s="1">
-        <v>15000</v>
+        <v>10500</v>
       </c>
       <c r="F155" s="1">
         <v>0</v>
@@ -3962,19 +4268,21 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
+        <f t="shared" si="4"/>
         <v>155</v>
       </c>
       <c r="B156" s="1">
+        <f t="shared" si="5"/>
         <v>155</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E156" s="1">
-        <v>11500</v>
+        <v>15000</v>
       </c>
       <c r="F156" s="1">
         <v>0</v>
@@ -3985,19 +4293,21 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
+        <f t="shared" si="4"/>
         <v>156</v>
       </c>
       <c r="B157" s="1">
+        <f t="shared" si="5"/>
         <v>156</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E157" s="1">
-        <v>11000</v>
+        <v>11500</v>
       </c>
       <c r="F157" s="1">
         <v>0</v>
@@ -4008,19 +4318,21 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
+        <f t="shared" si="4"/>
         <v>157</v>
       </c>
       <c r="B158" s="1">
+        <f t="shared" si="5"/>
         <v>157</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E158" s="1">
-        <v>13000</v>
+        <v>11000</v>
       </c>
       <c r="F158" s="1">
         <v>0</v>
@@ -4031,19 +4343,21 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
+        <f t="shared" si="4"/>
         <v>158</v>
       </c>
       <c r="B159" s="1">
+        <f t="shared" si="5"/>
         <v>158</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E159" s="1">
-        <v>10500</v>
+        <v>13000</v>
       </c>
       <c r="F159" s="1">
         <v>0</v>
@@ -4054,19 +4368,21 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
+        <f t="shared" si="4"/>
         <v>159</v>
       </c>
       <c r="B160" s="1">
+        <f t="shared" si="5"/>
         <v>159</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E160" s="1">
-        <v>15000</v>
+        <v>10500</v>
       </c>
       <c r="F160" s="1">
         <v>0</v>
@@ -4077,19 +4393,21 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
+        <f t="shared" si="4"/>
         <v>160</v>
       </c>
       <c r="B161" s="1">
+        <f t="shared" si="5"/>
         <v>160</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E161" s="1">
-        <v>11500</v>
+        <v>15000</v>
       </c>
       <c r="F161" s="1">
         <v>0</v>
@@ -4100,19 +4418,21 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
+        <f t="shared" si="4"/>
         <v>161</v>
       </c>
       <c r="B162" s="1">
+        <f t="shared" si="5"/>
         <v>161</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E162" s="1">
-        <v>35000</v>
+        <v>11500</v>
       </c>
       <c r="F162" s="1">
         <v>0</v>
@@ -4123,19 +4443,21 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
+        <f t="shared" si="4"/>
         <v>162</v>
       </c>
       <c r="B163" s="1">
+        <f t="shared" si="5"/>
         <v>162</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E163" s="1">
-        <v>34000</v>
+        <v>35000</v>
       </c>
       <c r="F163" s="1">
         <v>0</v>
@@ -4146,19 +4468,21 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
+        <f t="shared" si="4"/>
         <v>163</v>
       </c>
       <c r="B164" s="1">
+        <f t="shared" si="5"/>
         <v>163</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E164" s="1">
-        <v>30000</v>
+        <v>34000</v>
       </c>
       <c r="F164" s="1">
         <v>0</v>
@@ -4169,19 +4493,21 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
+        <f t="shared" si="4"/>
         <v>164</v>
       </c>
       <c r="B165" s="1">
+        <f t="shared" si="5"/>
         <v>164</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E165" s="1">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F165" s="1">
         <v>0</v>
@@ -4192,19 +4518,21 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
+        <f t="shared" si="4"/>
         <v>165</v>
       </c>
       <c r="B166" s="1">
+        <f t="shared" si="5"/>
         <v>165</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E166" s="1">
-        <v>35000</v>
+        <v>40000</v>
       </c>
       <c r="F166" s="1">
         <v>0</v>
@@ -4215,19 +4543,21 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
+        <f t="shared" si="4"/>
         <v>166</v>
       </c>
       <c r="B167" s="1">
+        <f t="shared" si="5"/>
         <v>166</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E167" s="1">
-        <v>34000</v>
+        <v>35000</v>
       </c>
       <c r="F167" s="1">
         <v>0</v>
@@ -4238,19 +4568,21 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
+        <f t="shared" si="4"/>
         <v>167</v>
       </c>
       <c r="B168" s="1">
+        <f t="shared" si="5"/>
         <v>167</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E168" s="1">
-        <v>10000</v>
+        <v>34000</v>
       </c>
       <c r="F168" s="1">
         <v>0</v>
@@ -4261,19 +4593,21 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
+        <f t="shared" si="4"/>
         <v>168</v>
       </c>
       <c r="B169" s="1">
+        <f t="shared" si="5"/>
         <v>168</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E169" s="1">
-        <v>11000</v>
+        <v>10000</v>
       </c>
       <c r="F169" s="1">
         <v>0</v>
@@ -4284,19 +4618,21 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
+        <f t="shared" si="4"/>
         <v>169</v>
       </c>
       <c r="B170" s="1">
+        <f t="shared" si="5"/>
         <v>169</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E170" s="1">
-        <v>13000</v>
+        <v>11000</v>
       </c>
       <c r="F170" s="1">
         <v>0</v>
@@ -4307,19 +4643,21 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
+        <f t="shared" si="4"/>
         <v>170</v>
       </c>
       <c r="B171" s="1">
+        <f t="shared" si="5"/>
         <v>170</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E171" s="1">
-        <v>10500</v>
+        <v>13000</v>
       </c>
       <c r="F171" s="1">
         <v>0</v>
@@ -4330,19 +4668,21 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
+        <f t="shared" si="4"/>
         <v>171</v>
       </c>
       <c r="B172" s="1">
+        <f t="shared" si="5"/>
         <v>171</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E172" s="1">
-        <v>15000</v>
+        <v>10500</v>
       </c>
       <c r="F172" s="1">
         <v>0</v>
@@ -4353,19 +4693,21 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
+        <f t="shared" si="4"/>
         <v>172</v>
       </c>
       <c r="B173" s="1">
+        <f t="shared" si="5"/>
         <v>172</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E173" s="1">
-        <v>11500</v>
+        <v>15000</v>
       </c>
       <c r="F173" s="1">
         <v>0</v>
@@ -4376,19 +4718,21 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
+        <f t="shared" si="4"/>
         <v>173</v>
       </c>
       <c r="B174" s="1">
+        <f t="shared" si="5"/>
         <v>173</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E174" s="1">
-        <v>11000</v>
+        <v>11500</v>
       </c>
       <c r="F174" s="1">
         <v>0</v>
@@ -4399,19 +4743,21 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
+        <f t="shared" si="4"/>
         <v>174</v>
       </c>
       <c r="B175" s="1">
+        <f t="shared" si="5"/>
         <v>174</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E175" s="1">
-        <v>13000</v>
+        <v>11000</v>
       </c>
       <c r="F175" s="1">
         <v>0</v>
@@ -4422,19 +4768,21 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
+        <f t="shared" si="4"/>
         <v>175</v>
       </c>
       <c r="B176" s="1">
+        <f t="shared" si="5"/>
         <v>175</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E176" s="1">
-        <v>10500</v>
+        <v>13000</v>
       </c>
       <c r="F176" s="1">
         <v>0</v>
@@ -4445,19 +4793,21 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
+        <f t="shared" si="4"/>
         <v>176</v>
       </c>
       <c r="B177" s="1">
+        <f t="shared" si="5"/>
         <v>176</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E177" s="1">
-        <v>15000</v>
+        <v>10500</v>
       </c>
       <c r="F177" s="1">
         <v>0</v>
@@ -4468,19 +4818,21 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
+        <f t="shared" si="4"/>
         <v>177</v>
       </c>
       <c r="B178" s="1">
+        <f t="shared" si="5"/>
         <v>177</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E178" s="1">
-        <v>11500</v>
+        <v>15000</v>
       </c>
       <c r="F178" s="1">
         <v>0</v>
@@ -4491,19 +4843,21 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
+        <f t="shared" si="4"/>
         <v>178</v>
       </c>
       <c r="B179" s="1">
+        <f t="shared" si="5"/>
         <v>178</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E179" s="1">
-        <v>35000</v>
+        <v>11500</v>
       </c>
       <c r="F179" s="1">
         <v>0</v>
@@ -4514,19 +4868,21 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
+        <f t="shared" si="4"/>
         <v>179</v>
       </c>
       <c r="B180" s="1">
+        <f t="shared" si="5"/>
         <v>179</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E180" s="1">
-        <v>34000</v>
+        <v>35000</v>
       </c>
       <c r="F180" s="1">
         <v>0</v>
@@ -4537,19 +4893,21 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
+        <f t="shared" si="4"/>
         <v>180</v>
       </c>
       <c r="B181" s="1">
+        <f t="shared" si="5"/>
         <v>180</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E181" s="1">
-        <v>25000</v>
+        <v>34000</v>
       </c>
       <c r="F181" s="1">
         <v>0</v>
@@ -4560,19 +4918,21 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
+        <f t="shared" si="4"/>
         <v>181</v>
       </c>
       <c r="B182" s="1">
+        <f t="shared" si="5"/>
         <v>181</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E182" s="1">
-        <v>27000</v>
+        <v>25000</v>
       </c>
       <c r="F182" s="1">
         <v>0</v>
@@ -4583,19 +4943,21 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
+        <f t="shared" si="4"/>
         <v>182</v>
       </c>
       <c r="B183" s="1">
+        <f t="shared" si="5"/>
         <v>182</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E183" s="1">
-        <v>29000</v>
+        <v>27000</v>
       </c>
       <c r="F183" s="1">
         <v>0</v>
@@ -4606,19 +4968,21 @@
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
+        <f t="shared" si="4"/>
         <v>183</v>
       </c>
       <c r="B184" s="1">
+        <f t="shared" si="5"/>
         <v>183</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E184" s="1">
-        <v>27007</v>
+        <v>29000</v>
       </c>
       <c r="F184" s="1">
         <v>0</v>
@@ -4629,19 +4993,21 @@
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
+        <f t="shared" si="4"/>
         <v>184</v>
       </c>
       <c r="B185" s="1">
+        <f t="shared" si="5"/>
         <v>184</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E185" s="1">
-        <v>27500</v>
+        <v>27007</v>
       </c>
       <c r="F185" s="1">
         <v>0</v>
@@ -4652,19 +5018,21 @@
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
+        <f t="shared" si="4"/>
         <v>185</v>
       </c>
       <c r="B186" s="1">
+        <f t="shared" si="5"/>
         <v>185</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E186" s="1">
-        <v>24890</v>
+        <v>27500</v>
       </c>
       <c r="F186" s="1">
         <v>0</v>
@@ -4675,19 +5043,21 @@
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
+        <f t="shared" si="4"/>
         <v>186</v>
       </c>
       <c r="B187" s="1">
+        <f t="shared" si="5"/>
         <v>186</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E187" s="1">
-        <v>22000</v>
+        <v>24890</v>
       </c>
       <c r="F187" s="1">
         <v>0</v>
@@ -4698,19 +5068,21 @@
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
+        <f t="shared" si="4"/>
         <v>187</v>
       </c>
       <c r="B188" s="1">
+        <f t="shared" si="5"/>
         <v>187</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E188" s="1">
-        <v>26589</v>
+        <v>22000</v>
       </c>
       <c r="F188" s="1">
         <v>0</v>
@@ -4721,22 +5093,24 @@
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
+        <f t="shared" si="4"/>
         <v>188</v>
       </c>
       <c r="B189" s="1">
+        <f t="shared" si="5"/>
         <v>188</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E189" s="1">
-        <v>3000</v>
+        <v>26589</v>
       </c>
       <c r="F189" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G189" s="1">
         <v>0</v>
@@ -4744,19 +5118,21 @@
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
+        <f t="shared" si="4"/>
         <v>189</v>
       </c>
       <c r="B190" s="1">
+        <f t="shared" si="5"/>
         <v>189</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E190" s="1">
-        <v>7700</v>
+        <v>3000</v>
       </c>
       <c r="F190" s="1">
         <v>1</v>
@@ -4767,19 +5143,21 @@
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
+        <f t="shared" si="4"/>
         <v>190</v>
       </c>
       <c r="B191" s="1">
+        <f t="shared" si="5"/>
         <v>190</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E191" s="1">
-        <v>7000</v>
+        <v>7700</v>
       </c>
       <c r="F191" s="1">
         <v>1</v>
@@ -4790,19 +5168,21 @@
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
+        <f t="shared" si="4"/>
         <v>191</v>
       </c>
       <c r="B192" s="1">
+        <f t="shared" si="5"/>
         <v>191</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E192" s="1">
-        <v>8000</v>
+        <v>7000</v>
       </c>
       <c r="F192" s="1">
         <v>1</v>
@@ -4813,19 +5193,21 @@
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
+        <f t="shared" si="4"/>
         <v>192</v>
       </c>
       <c r="B193" s="1">
+        <f t="shared" si="5"/>
         <v>192</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E193" s="1">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="F193" s="1">
         <v>1</v>
@@ -4836,19 +5218,21 @@
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
+        <f t="shared" si="4"/>
         <v>193</v>
       </c>
       <c r="B194" s="1">
+        <f t="shared" si="5"/>
         <v>193</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E194" s="1">
-        <v>8600</v>
+        <v>7500</v>
       </c>
       <c r="F194" s="1">
         <v>1</v>
@@ -4859,19 +5243,21 @@
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
+        <f t="shared" si="4"/>
         <v>194</v>
       </c>
       <c r="B195" s="1">
+        <f t="shared" si="5"/>
         <v>194</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E195" s="1">
-        <v>8000</v>
+        <v>8600</v>
       </c>
       <c r="F195" s="1">
         <v>1</v>
@@ -4882,19 +5268,21 @@
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
+        <f t="shared" ref="A196:A200" si="6">A195+1</f>
         <v>195</v>
       </c>
       <c r="B196" s="1">
+        <f t="shared" ref="B196:B200" si="7">B195+1</f>
         <v>195</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E196" s="1">
-        <v>9000</v>
+        <v>8000</v>
       </c>
       <c r="F196" s="1">
         <v>1</v>
@@ -4905,19 +5293,21 @@
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
+        <f t="shared" si="6"/>
         <v>196</v>
       </c>
       <c r="B197" s="1">
+        <f t="shared" si="7"/>
         <v>196</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E197" s="1">
-        <v>10000</v>
+        <v>9000</v>
       </c>
       <c r="F197" s="1">
         <v>1</v>
@@ -4928,19 +5318,21 @@
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
+        <f t="shared" si="6"/>
         <v>197</v>
       </c>
       <c r="B198" s="1">
+        <f t="shared" si="7"/>
         <v>197</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E198" s="1">
-        <v>11000</v>
+        <v>10000</v>
       </c>
       <c r="F198" s="1">
         <v>1</v>
@@ -4951,25 +5343,121 @@
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
+        <f t="shared" si="6"/>
         <v>198</v>
       </c>
       <c r="B199" s="1">
+        <f t="shared" si="7"/>
         <v>198</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E199" s="1">
+        <v>11000</v>
+      </c>
+      <c r="F199" s="1">
+        <v>1</v>
+      </c>
+      <c r="G199" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A200" s="1">
+        <f t="shared" si="6"/>
+        <v>199</v>
+      </c>
+      <c r="B200" s="1">
+        <f t="shared" si="7"/>
+        <v>199</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E200" s="1">
         <v>8000</v>
       </c>
-      <c r="F199" s="1">
-        <v>1</v>
-      </c>
-      <c r="G199" s="1">
-        <v>0</v>
+      <c r="F200" s="1">
+        <v>1</v>
+      </c>
+      <c r="G200" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A201" s="1">
+        <v>200</v>
+      </c>
+      <c r="B201" s="1">
+        <v>200</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E201" s="1">
+        <v>11000</v>
+      </c>
+      <c r="F201" s="1">
+        <v>1</v>
+      </c>
+      <c r="G201" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A202" s="1">
+        <v>201</v>
+      </c>
+      <c r="B202" s="1">
+        <v>201</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E202" s="1">
+        <v>8000</v>
+      </c>
+      <c r="F202" s="1">
+        <v>1</v>
+      </c>
+      <c r="G202" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A203" s="1">
+        <v>202</v>
+      </c>
+      <c r="B203" s="1">
+        <v>202</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E203" s="1">
+        <v>11000</v>
+      </c>
+      <c r="F203" s="1">
+        <v>1</v>
+      </c>
+      <c r="G203" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed model to correct p-value for gender
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonly\Documents\GitHub\prescription-fill-prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D2EFA3-F9F9-4500-89AE-CBF19029A080}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC9C571-4012-49B9-96DB-8157FDC9DEDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -376,12 +376,36 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="6">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{5E1A3C4E-4CD2-4E7B-BE2C-E43C5F0DCFD6}">
+  <we:reference id="wa104379190" version="2.0.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa104379190" version="2.0.0.0" store="WA104379190" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings>
+    <we:binding id="RangeSelect" type="matrix" appref="{04B20FBD-D524-4E90-A90F-B12F8A2C0B28}"/>
+    <we:binding id="InputY" type="matrix" appref="{B9D90BE5-B92F-4945-998F-66427871B349}"/>
+    <we:binding id="InputX" type="matrix" appref="{DA2D1BF4-5ED9-43BA-B5D6-DC03B2114529}"/>
+  </we:bindings>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="K203" sqref="K203"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5462,5 +5486,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{F7C9EE02-42E1-4005-9D12-6889AFFD525C}">
+      <x15:webExtensions xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x15:webExtension appRef="{04B20FBD-D524-4E90-A90F-B12F8A2C0B28}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{B9D90BE5-B92F-4945-998F-66427871B349}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{DA2D1BF4-5ED9-43BA-B5D6-DC03B2114529}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+      </x15:webExtensions>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>